<commit_message>
removed url from xl
</commit_message>
<xml_diff>
--- a/CTDC_Automation/InputFiles/TC01_Canine_Filter_Study-COTB.xlsx
+++ b/CTDC_Automation/InputFiles/TC01_Canine_Filter_Study-COTB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Script\DataCommons_Automation\CTDC_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE572A4-F16E-4760-B3C3-2B875355F819}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096756E4-377D-4CDE-A5FA-8BAC53E1C74C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,13 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>https://caninecommons.cancer.gov/#/</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>WebExcel</t>
   </si>
@@ -48,31 +42,23 @@
     <t>dbExcel</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE s.clinical_study_designation IN ['COTC007B'] WITH DISTINCT c AS c, p, s, demo, diag RETURN coalesce(c.case_id,'') AS case_id , coalesce(s.clinical_study_designation,'') AS study_code , coalesce(s.clinical_study_type,'') AS study_type , coalesce(demo.breed,'') AS breed , coalesce(diag.disease_term,'') AS diagnosis , coalesce(diag.stage_of_disease,'') AS stage_of_disease , coalesce(demo.patient_age_at_enrollment,'') AS age , coalesce(demo.sex,'') AS sex , coalesce(demo.neutered_indicator,'') AS neutered_status</t>
-  </si>
-  <si>
     <t>TC01_Canine_Filter_Study-COTB_Neo4jData.xlsx</t>
   </si>
   <si>
     <t>TC01_Canine_Filter_Study-COTB_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE s.clinical_study_designation IN ['COTC007B'] WITH DISTINCT c AS c, p, s, demo, diag RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(s.clinical_study_designation,'') AS `Study Code` , coalesce(s.clinical_study_type,'') AS  `Study Type`, coalesce(demo.breed,'') AS Breed , coalesce(diag.disease_term,'') AS Diagnosis , coalesce(diag.stage_of_disease,'') AS `Stage of Disease` ,  coalesce(demo.patient_age_at_enrollment,'') AS Age , coalesce(demo.sex,'') AS Sex , coalesce(demo.neutered_indicator,'') AS  `Neutered Status`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,22 +94,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{7EA68BB1-159D-4F44-96A3-D0B7FBE8815D}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{7EA68BB1-159D-4F44-96A3-D0B7FBE8815D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,54 +418,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75.81640625" customWidth="1"/>
+    <col min="2" max="2" width="70.26953125" customWidth="1"/>
+    <col min="3" max="3" width="39.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="174" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="/" xr:uid="{EE6720A7-C9D8-4EE2-8E31-C0EFEB18C846}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>